<commit_message>
fix Vinzor & lab03test.xlsx after lection 04.12.16
</commit_message>
<xml_diff>
--- a/labs/lab03test.xlsx
+++ b/labs/lab03test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9780"/>
+    <workbookView xWindow="240" yWindow="132" windowWidth="21072" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t xml:space="preserve"> DW =</t>
   </si>
   <si>
-    <t>Автокоррел. (1-отсутств.;2-положит;3-отриц) =</t>
-  </si>
-  <si>
     <t>Показатель сист. влияния, a =</t>
   </si>
   <si>
@@ -395,6 +392,9 @@
   </si>
   <si>
     <t>Критич. знач. t-статистики Стьюдента, t =</t>
+  </si>
+  <si>
+    <t>Автокоррел. (1-отсутств.;2-положит;3-отриц;4-ненадёж.) =</t>
   </si>
 </sst>
 </file>
@@ -898,21 +898,21 @@
   <dimension ref="A1:IV32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="62.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="66.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="256" width="0" hidden="1" customWidth="1"/>
-    <col min="257" max="16384" width="9.140625" hidden="1"/>
+    <col min="257" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="18.75">
+    <row r="1" spans="1:256" ht="17.399999999999999">
       <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
@@ -1172,7 +1172,7 @@
       <c r="IU1" s="9"/>
       <c r="IV1" s="9"/>
     </row>
-    <row r="2" spans="1:256" ht="18.75">
+    <row r="2" spans="1:256" ht="18">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1183,7 +1183,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:256" ht="20.25">
+    <row r="3" spans="1:256" ht="20.399999999999999">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1196,18 +1196,18 @@
       <c r="D3" s="5"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:256" ht="18.75">
+    <row r="4" spans="1:256" ht="18">
       <c r="A4" s="10">
         <v>2</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:256" ht="20.25">
+    <row r="5" spans="1:256" ht="20.399999999999999">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -1218,18 +1218,18 @@
       <c r="D5" s="5"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:256" ht="18.75">
+    <row r="6" spans="1:256" ht="18">
       <c r="A6" s="10">
         <v>4</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:256" ht="18.75">
+    <row r="7" spans="1:256" ht="18">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:256" ht="18.75">
+    <row r="8" spans="1:256" ht="18">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1253,62 +1253,62 @@
       <c r="D8" s="5"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:256" ht="20.25">
+    <row r="9" spans="1:256" ht="20.399999999999999">
       <c r="A9" s="10">
         <v>7</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:256" ht="20.25">
+    <row r="10" spans="1:256" ht="20.399999999999999">
       <c r="A10" s="10">
         <v>8</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:256" ht="20.25">
+    <row r="11" spans="1:256" ht="20.399999999999999">
       <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="20.25">
+    <row r="12" spans="1:256" ht="20.399999999999999">
       <c r="A12" s="10">
         <v>10</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:256" ht="23.25">
+    <row r="13" spans="1:256" ht="21.6">
       <c r="A13" s="10">
         <v>11</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="20.25">
+    <row r="14" spans="1:256" ht="20.399999999999999">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:256" ht="20.25">
+    <row r="15" spans="1:256" ht="20.399999999999999">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -1330,18 +1330,18 @@
       <c r="D15" s="5"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:256" ht="18.75">
+    <row r="16" spans="1:256" ht="18">
       <c r="A16" s="10">
         <v>14</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="18.75">
+    <row r="17" spans="1:5" ht="18">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -1352,7 +1352,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="18.75">
+    <row r="18" spans="1:5" ht="18">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -1360,12 +1360,12 @@
         <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="18.75">
+    <row r="19" spans="1:5" ht="18">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="D19" s="7"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" ht="20.25">
+    <row r="20" spans="1:5" ht="20.399999999999999">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -1387,7 +1387,7 @@
       <c r="D20" s="7"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" ht="20.25">
+    <row r="21" spans="1:5" ht="20.399999999999999">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" ht="18.75">
+    <row r="22" spans="1:5" ht="18">
       <c r="A22" s="10">
         <v>20</v>
       </c>
@@ -1409,7 +1409,7 @@
       <c r="D22" s="7"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" ht="18.75">
+    <row r="23" spans="1:5" ht="18">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="D23" s="5"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="18.75">
+    <row r="24" spans="1:5" ht="18">
       <c r="A24" s="10">
         <v>22</v>
       </c>
@@ -1433,7 +1433,7 @@
       <c r="D24" s="5"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="20.25">
+    <row r="25" spans="1:5" ht="20.399999999999999">
       <c r="A25" s="10">
         <v>23</v>
       </c>
@@ -1444,7 +1444,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="20.25">
+    <row r="26" spans="1:5" ht="20.399999999999999">
       <c r="A26" s="10">
         <v>24</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="D26" s="5"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="18.75">
+    <row r="27" spans="1:5" ht="18">
       <c r="A27" s="10">
         <v>25</v>
       </c>
@@ -1479,35 +1479,35 @@
       <c r="D28" s="5"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="18.75">
+    <row r="29" spans="1:5" ht="18">
       <c r="A29" s="10">
         <v>27</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="18.75">
+    <row r="30" spans="1:5" ht="18">
       <c r="A30" s="10">
         <v>28</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="18.75">
+    <row r="31" spans="1:5" ht="18">
       <c r="A31" s="10">
         <v>29</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="3"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="3"/>
@@ -1545,7 +1545,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1557,7 +1557,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>